<commit_message>
Creation of demonstration example
</commit_message>
<xml_diff>
--- a/reference/tests/input1_population_and_period.xlsx
+++ b/reference/tests/input1_population_and_period.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\corp.ssi.govt.nz\userss\sanas001\Documents\Simon's Documents\GDAT tool\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon &amp; Izzi\Documents\Simon\Projects\Current projects\idi_tool_packages\reference\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF55BB2-9F02-45CE-B128-1932EE745AAC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,9 +35,6 @@
     <t>Schema_name</t>
   </si>
   <si>
-    <t>[DL-MAA2016-15]</t>
-  </si>
-  <si>
     <t>Table_name</t>
   </si>
   <si>
@@ -82,12 +78,15 @@
   </si>
   <si>
     <t>"registration to appointment"</t>
+  </si>
+  <si>
+    <t>[DL-MAA20XX-YY]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -398,11 +397,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,22 +424,22 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
       <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
         <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -448,25 +447,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -474,25 +473,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>